<commit_message>
updated with spdsw_r23022_2017-03-23 by cron
</commit_message>
<xml_diff>
--- a/idl/projects/themis/ground/THEMIS_GMAG_Station_List_Jan_2017.xlsx
+++ b/idl/projects/themis/ground/THEMIS_GMAG_Station_List_Jan_2017.xlsx
@@ -2684,8 +2684,8 @@
   </sheetPr>
   <dimension ref="A1:AC174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y149" sqref="Y149"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q66" sqref="Q66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6249,7 +6249,7 @@
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="11">
-        <v>68.5</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="R66" s="11">
         <v>27.29</v>

</xml_diff>